<commit_message>
update showcase model transfer script
</commit_message>
<xml_diff>
--- a/gropin/showcase/showcase_MD.xlsx
+++ b/gropin/showcase/showcase_MD.xlsx
@@ -632,7 +632,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Gropin Model Nr. 24</t>
+          <t>Gropin growth model for Aeromonas hydrophila in/on modified BHI (gropin ID: 24 )</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>15.10.2020</t>
+          <t>15/10/2020</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="O133" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'responsesurface' or 'time2multiply'. Environmental factors for growth model.</t>
         </is>
       </c>
       <c r="P133" t="inlineStr">
@@ -5339,22 +5339,7 @@
       </c>
       <c r="R133" t="inlineStr">
         <is>
-          <t>double</t>
-        </is>
-      </c>
-      <c r="S133" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T133" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U133" t="inlineStr">
-        <is>
-          <t>mydist</t>
+          <t>DOUBLE</t>
         </is>
       </c>
       <c r="V133" t="inlineStr">
@@ -5401,7 +5386,7 @@
       </c>
       <c r="O134" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'responsesurface' or 'time2multiply'. Environmental factors for growth model.</t>
         </is>
       </c>
       <c r="P134" t="inlineStr">
@@ -5416,22 +5401,7 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>double</t>
-        </is>
-      </c>
-      <c r="S134" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T134" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U134" t="inlineStr">
-        <is>
-          <t>mydist</t>
+          <t>DOUBLE</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
@@ -5473,7 +5443,7 @@
       </c>
       <c r="O135" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'responsesurface' or 'time2multiply'. Environmental factors for growth model.</t>
         </is>
       </c>
       <c r="P135" t="inlineStr">
@@ -5488,22 +5458,7 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>double</t>
-        </is>
-      </c>
-      <c r="S135" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T135" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U135" t="inlineStr">
-        <is>
-          <t>mydist</t>
+          <t>DOUBLE</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
@@ -5543,11 +5498,6 @@
           <t>b</t>
         </is>
       </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>my dummy description</t>
-        </is>
-      </c>
       <c r="P136" t="inlineStr">
         <is>
           <t>[]</t>
@@ -5561,21 +5511,6 @@
       <c r="R136" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T136" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
@@ -5620,11 +5555,6 @@
           <t>awmin</t>
         </is>
       </c>
-      <c r="O137" t="inlineStr">
-        <is>
-          <t>my dummy description</t>
-        </is>
-      </c>
       <c r="P137" t="inlineStr">
         <is>
           <t>[]</t>
@@ -5638,21 +5568,6 @@
       <c r="R137" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S137" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T137" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U137" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
@@ -5692,11 +5607,6 @@
           <t>Tmin</t>
         </is>
       </c>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>my dummy description</t>
-        </is>
-      </c>
       <c r="P138" t="inlineStr">
         <is>
           <t>[]</t>
@@ -5710,21 +5620,6 @@
       <c r="R138" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S138" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T138" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U138" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V138" t="inlineStr">
@@ -5764,11 +5659,6 @@
           <t>CO2max</t>
         </is>
       </c>
-      <c r="O139" t="inlineStr">
-        <is>
-          <t>my dummy description</t>
-        </is>
-      </c>
       <c r="P139" t="inlineStr">
         <is>
           <t>[]</t>
@@ -5782,21 +5672,6 @@
       <c r="R139" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S139" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T139" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U139" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V139" t="inlineStr">
@@ -5853,7 +5728,7 @@
       </c>
       <c r="O140" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>For visualisation purposes in either mode 'time2multiply' or 'responsesurface'. visualisation axis. Enter string with '&lt;variable ID&gt;'. Strings that are accepted: T, aw, CO2dissolved</t>
         </is>
       </c>
       <c r="P140" t="inlineStr">
@@ -5869,21 +5744,6 @@
       <c r="R140" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S140" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T140" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U140" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
@@ -5930,7 +5790,7 @@
       </c>
       <c r="O141" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>For visualisation purposes in either mode 'time2multiply' or 'responsesurface'. visualisation axis. Enter string with '&lt;variable ID&gt;'. Strings that are accepted: T, aw, CO2dissolved</t>
         </is>
       </c>
       <c r="P141" t="inlineStr">
@@ -5946,21 +5806,6 @@
       <c r="R141" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S141" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T141" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U141" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V141" t="inlineStr">
@@ -6017,7 +5862,7 @@
       </c>
       <c r="O142" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>three different modes are available: 'responsesurface' is running the secondary model calculating mumax only. 'time2multiply' returns a 2D-plot of the time the microorganism needs to increase N by a logstep of 'logIncrease'(free parameter to choose). 'kinetic' runs the tertiary model, based on the variables chosen (with '_kinetic'-suffix).</t>
         </is>
       </c>
       <c r="P142" t="inlineStr">
@@ -6033,21 +5878,6 @@
       <c r="R142" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S142" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T142" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U142" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V142" t="inlineStr">
@@ -6094,7 +5924,7 @@
       </c>
       <c r="O143" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'time2multiply' or 'kinetic' is chosen. This is the time the microorganism needs for adjusting to its environment before multiplying.</t>
         </is>
       </c>
       <c r="P143" t="inlineStr">
@@ -6110,21 +5940,6 @@
       <c r="R143" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S143" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T143" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U143" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V143" t="inlineStr">
@@ -6156,7 +5971,7 @@
       </c>
       <c r="O144" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in mode 'time2multiply'. Free parameter to calculate the time the microorganism needs to increase its numbers by the log step increase indictated by this value.</t>
         </is>
       </c>
       <c r="P144" t="inlineStr">
@@ -6172,21 +5987,6 @@
       <c r="R144" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S144" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T144" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U144" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V144" t="inlineStr">
@@ -6218,7 +6018,7 @@
       </c>
       <c r="O145" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'kinetic'. Choose the number of microorganisms at the beginning of this simulation. (log step!)</t>
         </is>
       </c>
       <c r="P145" t="inlineStr">
@@ -6234,21 +6034,6 @@
       <c r="R145" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S145" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T145" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U145" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V145" t="inlineStr">
@@ -6280,7 +6065,7 @@
       </c>
       <c r="O146" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'kinetic'. Choose the number of microorganisms at the end of this simulation. (log step!)</t>
         </is>
       </c>
       <c r="P146" t="inlineStr">
@@ -6296,21 +6081,6 @@
       <c r="R146" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S146" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T146" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U146" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V146" t="inlineStr">
@@ -6357,7 +6127,7 @@
       </c>
       <c r="O147" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>time of simulation, unit is h-1</t>
         </is>
       </c>
       <c r="P147" t="inlineStr">
@@ -6373,21 +6143,6 @@
       <c r="R147" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S147" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T147" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U147" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V147" t="inlineStr">
@@ -6434,7 +6189,7 @@
       </c>
       <c r="O148" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'kinetic'. Choose variable for prediction of growth depending on environmental factors.</t>
         </is>
       </c>
       <c r="P148" t="inlineStr">
@@ -6450,21 +6205,6 @@
       <c r="R148" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S148" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T148" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U148" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V148" t="inlineStr">
@@ -6511,7 +6251,7 @@
       </c>
       <c r="O149" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'kinetic'. Choose variable for prediction of growth depending on environmental factors.</t>
         </is>
       </c>
       <c r="P149" t="inlineStr">
@@ -6527,21 +6267,6 @@
       <c r="R149" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S149" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T149" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U149" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V149" t="inlineStr">
@@ -6589,7 +6314,7 @@
       </c>
       <c r="O150" t="inlineStr">
         <is>
-          <t>my dummy description</t>
+          <t>Only applicaple in either mode 'kinetic'. Choose variable for prediction of growth depending on environmental factors.</t>
         </is>
       </c>
       <c r="P150" t="inlineStr">
@@ -6605,21 +6330,6 @@
       <c r="R150" t="inlineStr">
         <is>
           <t>double</t>
-        </is>
-      </c>
-      <c r="S150" t="inlineStr">
-        <is>
-          <t>my source</t>
-        </is>
-      </c>
-      <c r="T150" t="inlineStr">
-        <is>
-          <t>my subject</t>
-        </is>
-      </c>
-      <c r="U150" t="inlineStr">
-        <is>
-          <t>mydist</t>
         </is>
       </c>
       <c r="V150" t="inlineStr">

</xml_diff>